<commit_message>
Added the chunked anonymization function
</commit_message>
<xml_diff>
--- a/ACCOUNTS UPSIDE.xlsx
+++ b/ACCOUNTS UPSIDE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopalmiero/Documents/Uni/Ricerca/UPSIDE/UPSIDE_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B87BBAF-ED1A-FC4B-9FB3-4046F7F5C87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D9F478-E086-BF48-8213-0AB5798EAE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="62">
   <si>
     <t>Fortnite Deathmatch</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>(Un)used IPs</t>
+  </si>
+  <si>
+    <t>192.168.0.8</t>
+  </si>
+  <si>
+    <t>192.168.0.33</t>
   </si>
 </sst>
 </file>
@@ -314,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -551,11 +557,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -633,14 +663,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,8 +682,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="161" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -894,7 +926,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
-      <c r="H2" s="32"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B3" s="1" t="s">
@@ -912,10 +944,10 @@
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="32"/>
+      <c r="H3" s="35"/>
       <c r="J3" s="29" t="s">
         <v>59</v>
       </c>
@@ -1126,15 +1158,15 @@
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B14" s="1" t="s">
@@ -1152,10 +1184,10 @@
       <c r="F14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="32"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" customHeight="1" thickTop="1">
       <c r="B15" s="4">
@@ -1267,7 +1299,7 @@
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
-      <c r="H20" s="32"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21" s="1" t="s">
@@ -1285,7 +1317,7 @@
       <c r="F21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="34"/>
@@ -1438,8 +1470,8 @@
       <c r="H26" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="28" t="s">
-        <v>51</v>
+      <c r="I26" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
@@ -1468,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -1500,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
@@ -1528,7 +1560,9 @@
       <c r="H29" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="28"/>
+      <c r="I29" s="28" t="s">
+        <v>57</v>
+      </c>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -1543,15 +1577,15 @@
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B32" s="1" t="s">
@@ -1569,7 +1603,7 @@
       <c r="F32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="34"/>
@@ -1597,7 +1631,7 @@
       <c r="H33" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="31" t="s">
         <v>26</v>
       </c>
       <c r="K33" s="16"/>
@@ -1624,8 +1658,8 @@
       <c r="H34" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I34" s="28" t="s">
-        <v>29</v>
+      <c r="I34" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="K34" s="16"/>
       <c r="L34" s="16"/>
@@ -1651,8 +1685,8 @@
       <c r="H35" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I35" s="28" t="s">
-        <v>31</v>
+      <c r="I35" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
@@ -1678,8 +1712,8 @@
       <c r="H36" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I36" s="28" t="s">
-        <v>34</v>
+      <c r="I36" s="42" t="s">
+        <v>31</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
@@ -1705,8 +1739,8 @@
       <c r="H37" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="28" t="s">
-        <v>45</v>
+      <c r="I37" s="42" t="s">
+        <v>34</v>
       </c>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
@@ -1732,8 +1766,8 @@
       <c r="H38" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I38" s="28" t="s">
-        <v>46</v>
+      <c r="I38" s="42" t="s">
+        <v>45</v>
       </c>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
@@ -1759,8 +1793,8 @@
       <c r="H39" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I39" s="28" t="s">
-        <v>49</v>
+      <c r="I39" s="42" t="s">
+        <v>46</v>
       </c>
       <c r="K39" s="16"/>
       <c r="L39" s="16"/>
@@ -1786,7 +1820,9 @@
       <c r="H40" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="I40" s="28"/>
+      <c r="I40" s="42" t="s">
+        <v>49</v>
+      </c>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
@@ -1809,7 +1845,7 @@
       <c r="E42" s="34"/>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
-      <c r="H42" s="32"/>
+      <c r="H42" s="35"/>
     </row>
     <row r="43" spans="2:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B43" s="1" t="s">
@@ -1827,10 +1863,10 @@
       <c r="F43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="31" t="s">
+      <c r="G43" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="32"/>
+      <c r="H43" s="35"/>
       <c r="I43" s="29" t="s">
         <v>23</v>
       </c>
@@ -1857,7 +1893,7 @@
       <c r="H44" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I44" s="40" t="s">
+      <c r="I44" s="31" t="s">
         <v>27</v>
       </c>
       <c r="L44" s="16"/>
@@ -1885,7 +1921,7 @@
       <c r="H45" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I45" s="40" t="s">
+      <c r="I45" s="31" t="s">
         <v>47</v>
       </c>
       <c r="L45" s="16"/>
@@ -1913,7 +1949,7 @@
       <c r="H46" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I46" s="40" t="s">
+      <c r="I46" s="31" t="s">
         <v>50</v>
       </c>
       <c r="L46" s="16"/>
@@ -1941,7 +1977,7 @@
       <c r="H47" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="I47" s="31" t="s">
         <v>56</v>
       </c>
       <c r="L47" s="16"/>
@@ -1965,7 +2001,7 @@
       <c r="E49" s="34"/>
       <c r="F49" s="34"/>
       <c r="G49" s="34"/>
-      <c r="H49" s="32"/>
+      <c r="H49" s="35"/>
     </row>
     <row r="50" spans="2:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B50" s="1" t="s">
@@ -1983,7 +2019,7 @@
       <c r="F50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H50" s="34"/>
@@ -2013,7 +2049,7 @@
       <c r="H51" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I51" s="41" t="s">
+      <c r="I51" s="32" t="s">
         <v>30</v>
       </c>
       <c r="K51" s="16"/>
@@ -2042,7 +2078,7 @@
       <c r="H52" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I52" s="40" t="s">
+      <c r="I52" s="31" t="s">
         <v>37</v>
       </c>
       <c r="K52" s="16"/>
@@ -2117,15 +2153,15 @@
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="2:13" ht="19">
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="37"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="39"/>
     </row>
     <row r="57" spans="2:13" ht="15" thickTop="1" thickBot="1">
       <c r="B57" s="1" t="s">
@@ -2143,10 +2179,10 @@
       <c r="F57" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="32"/>
+      <c r="H57" s="35"/>
       <c r="I57" s="29" t="s">
         <v>23</v>
       </c>
@@ -2411,10 +2447,10 @@
       <c r="F68" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G68" s="38" t="s">
+      <c r="G68" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H68" s="39"/>
+      <c r="H68" s="41"/>
     </row>
     <row r="69" spans="2:13" ht="14" thickTop="1">
       <c r="B69" s="4">
@@ -2594,15 +2630,15 @@
       <c r="H77" s="12"/>
     </row>
     <row r="78" spans="2:13" ht="19">
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="37"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="39"/>
     </row>
     <row r="79" spans="2:13" ht="15" thickTop="1" thickBot="1">
       <c r="B79" s="1" t="s">
@@ -2620,10 +2656,10 @@
       <c r="F79" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G79" s="31" t="s">
+      <c r="G79" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H79" s="32"/>
+      <c r="H79" s="35"/>
     </row>
     <row r="80" spans="2:13" ht="14" thickTop="1">
       <c r="B80" s="4">
@@ -2723,16 +2759,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="B78:H78"/>
     <mergeCell ref="G79:H79"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="B42:H42"/>
@@ -2741,6 +2767,16 @@
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="B56:H56"/>
     <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="B78:H78"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B20:H20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>